<commit_message>
actualización de Entregable 2 RF-16
Se llega hasta la referencia 16, modulo de Consulta de documentos
</commit_message>
<xml_diff>
--- a/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
+++ b/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROYECTO_SIGEDOC\SIGEDOC\Documentacion\Entregables Para Henry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF30B8CB-06B2-4183-85DF-A3AED979E7C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF2ABE7-18CB-425B-85F4-992A166D8368}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05819A6B-DF8F-4A1E-9F97-98F9155DCADB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>REQUERIMIENTO</t>
   </si>
@@ -42,24 +42,12 @@
     <t>OBJETOS</t>
   </si>
   <si>
-    <t>Menu Principal</t>
-  </si>
-  <si>
     <t>DAVIVIENDA</t>
   </si>
   <si>
     <t>CR38010400141526566616</t>
   </si>
   <si>
-    <t>VIDAL Jimenez Rojas</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>Centro de Costos</t>
-  </si>
-  <si>
     <t>Fecha y Hora Actual</t>
   </si>
   <si>
@@ -72,46 +60,71 @@
     <t>Rol Asignado</t>
   </si>
   <si>
-    <t>RF-06</t>
-  </si>
-  <si>
-    <t>Nombre del documento</t>
-  </si>
-  <si>
-    <t>Asunto</t>
-  </si>
-  <si>
-    <t>usuario</t>
-  </si>
-  <si>
-    <t>Numero de Referencia</t>
-  </si>
-  <si>
-    <t>Status del documento</t>
-  </si>
-  <si>
-    <t>Caja de texto con la informacion del proyecto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lista de documentos </t>
-  </si>
-  <si>
-    <t>Boton Crear Nuevo Documento</t>
-  </si>
-  <si>
-    <t>Boton Subir documento recibido</t>
-  </si>
-  <si>
-    <t>Ver detalles se obtiene un pagina con toda la información necesaria del sistema, y se encontrara en detalle la información del proyecto y una lista con referencia de cada documento subido y creado al proyecto en revisión, en esta sección se cuentan con dos opciones:
-• Crear Documento
-• Subir documento Recibido.</t>
+    <t>RF-09</t>
+  </si>
+  <si>
+    <t>En la opción de cargar documento , encontramos un boton donde a la hora de subir un documento previamnete diseñado por la creacion del machote, en este el usuario indicara si es firma digital o firma manual, si es firma digital este valida si existe la firma digital, en caso de no existir la firma tendra un aviso de que no hay firma digital lo cual sera un paso necesario para poder subir el docuemnto en formato pdf, si la firma es manual solamente se validara si el docuemnto es en pdf</t>
+  </si>
+  <si>
+    <t>Menú Principal</t>
+  </si>
+  <si>
+    <t>Nombre Cliente</t>
+  </si>
+  <si>
+    <t>Nombre de la persona de contacto</t>
+  </si>
+  <si>
+    <t>Numero de Teléfono</t>
+  </si>
+  <si>
+    <t>Correo Electronico</t>
+  </si>
+  <si>
+    <t>observaciones</t>
+  </si>
+  <si>
+    <t>Botón registrar</t>
+  </si>
+  <si>
+    <t>Boton Descartar</t>
+  </si>
+  <si>
+    <t>RF-16</t>
+  </si>
+  <si>
+    <t>En esta sección se contará con toda la información del sistema, además contará con filtros para buscar documentos de acuerdo con su número de registro, centro de costos, año, cliente, y tendrá las siguientes opciones:</t>
+  </si>
+  <si>
+    <t>Filto numero referencia</t>
+  </si>
+  <si>
+    <t>Filtro Año</t>
+  </si>
+  <si>
+    <t>Filtro Centro Costos</t>
+  </si>
+  <si>
+    <t>Filtro Cliente</t>
+  </si>
+  <si>
+    <t>Filtro Proyecto</t>
+  </si>
+  <si>
+    <t>Lista de documentos</t>
+  </si>
+  <si>
+    <t>Ver detalles</t>
+  </si>
+  <si>
+    <t>Modificar detalles del documento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +136,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,11 +183,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,13 +199,31 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,219 +539,394 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2F3CCD-3DE1-4D13-AD96-4E84CCAA0BEB}">
-  <dimension ref="B2:K30"/>
+  <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="H3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="4" spans="2:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="H5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="H6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="H7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="H9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="H11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="H12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="2:6" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="H13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>4</v>
       </c>
-      <c r="G30" t="s">
-        <v>5</v>
-      </c>
-      <c r="I30" t="s">
-        <v>6</v>
-      </c>
-      <c r="K30">
-        <v>1570967</v>
+      <c r="L30" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="40">
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C19:F19"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
@@ -730,10 +940,6 @@
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="C5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion Entregable 2 RF-21
Se actualiza a la Referencia 21
</commit_message>
<xml_diff>
--- a/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
+++ b/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROYECTO_SIGEDOC\SIGEDOC\Documentacion\Entregables Para Henry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF2ABE7-18CB-425B-85F4-992A166D8368}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C2C3E6-1866-4738-8B7A-915992657CAC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05819A6B-DF8F-4A1E-9F97-98F9155DCADB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>REQUERIMIENTO</t>
   </si>
@@ -90,34 +90,13 @@
     <t>Boton Descartar</t>
   </si>
   <si>
-    <t>RF-16</t>
-  </si>
-  <si>
-    <t>En esta sección se contará con toda la información del sistema, además contará con filtros para buscar documentos de acuerdo con su número de registro, centro de costos, año, cliente, y tendrá las siguientes opciones:</t>
-  </si>
-  <si>
-    <t>Filto numero referencia</t>
-  </si>
-  <si>
-    <t>Filtro Año</t>
-  </si>
-  <si>
-    <t>Filtro Centro Costos</t>
-  </si>
-  <si>
-    <t>Filtro Cliente</t>
-  </si>
-  <si>
-    <t>Filtro Proyecto</t>
-  </si>
-  <si>
-    <t>Lista de documentos</t>
-  </si>
-  <si>
-    <t>Ver detalles</t>
-  </si>
-  <si>
-    <t>Modificar detalles del documento</t>
+    <t>RF-23</t>
+  </si>
+  <si>
+    <t>En esta sección se contará con toda la información del sistema, aparte contara con una opcion de dar de baja al usuario, lo cual el sistema no permitiria mas su ingreso, pero no se elimina ya que el usuario estara registrado en reportes y actividades que haya realizado.</t>
+  </si>
+  <si>
+    <t>Dar de Baja</t>
   </si>
 </sst>
 </file>
@@ -156,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -179,11 +158,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -201,29 +206,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2F3CCD-3DE1-4D13-AD96-4E84CCAA0BEB}">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,307 +577,293 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
       <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="H3" s="10" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="H3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="2:12" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
       <c r="H5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
     </row>
     <row r="6" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
       <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
     </row>
     <row r="7" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
       <c r="H7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="H8" s="13" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="H8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
       <c r="H9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="H10" s="13" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="H10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="2:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
       <c r="H11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
     </row>
     <row r="12" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="H13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
     </row>
     <row r="15" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
     </row>
     <row r="16" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
     </row>
     <row r="17" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
     </row>
     <row r="18" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
     </row>
     <row r="19" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
     </row>
     <row r="21" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
@@ -900,28 +906,8 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:F4"/>
@@ -938,8 +924,28 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Ultima actualización del documento #2
Esta a aun 90% de terminado
</commit_message>
<xml_diff>
--- a/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
+++ b/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROYECTO_SIGEDOC\SIGEDOC\Documentacion\Entregables Para Henry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44151EFA-A4A4-4496-BB0F-B8BFE2A25A0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037A64D7-EB66-4B7D-B978-4400BF8D7C3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05819A6B-DF8F-4A1E-9F97-98F9155DCADB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>REQUERIMIENTO</t>
   </si>
@@ -54,36 +54,9 @@
     <t>Nombre y apellido del usuario</t>
   </si>
   <si>
-    <t>RF-09</t>
-  </si>
-  <si>
-    <t>En la opción de cargar documento , encontramos un boton donde a la hora de subir un documento previamnete diseñado por la creacion del machote, en este el usuario indicara si es firma digital o firma manual, si es firma digital este valida si existe la firma digital, en caso de no existir la firma tendra un aviso de que no hay firma digital lo cual sera un paso necesario para poder subir el docuemnto en formato pdf, si la firma es manual solamente se validara si el docuemnto es en pdf</t>
-  </si>
-  <si>
     <t>Menú Principal</t>
   </si>
   <si>
-    <t>Nombre Cliente</t>
-  </si>
-  <si>
-    <t>Nombre de la persona de contacto</t>
-  </si>
-  <si>
-    <t>Numero de Teléfono</t>
-  </si>
-  <si>
-    <t>Correo Electronico</t>
-  </si>
-  <si>
-    <t>observaciones</t>
-  </si>
-  <si>
-    <t>Botón registrar</t>
-  </si>
-  <si>
-    <t>Boton Descartar</t>
-  </si>
-  <si>
     <t>Título del sistema</t>
   </si>
   <si>
@@ -100,6 +73,27 @@
   </si>
   <si>
     <t>Reporte Auditoria</t>
+  </si>
+  <si>
+    <t>RF-26
+Roles</t>
+  </si>
+  <si>
+    <t>En esta sección se contará con toda la información del sistema, aparte contara con el registro de roles y permisos con los que contará el usuario que ingresara al sistema, Cuenta con dos opciones:
+• Crear nuevo rol. 
+• Consultar rol.</t>
+  </si>
+  <si>
+    <t>Fecha y hora Actual</t>
+  </si>
+  <si>
+    <t>Menú principal</t>
+  </si>
+  <si>
+    <t>Crear nuevo Rol</t>
+  </si>
+  <si>
+    <t>Consultar rol</t>
   </si>
 </sst>
 </file>
@@ -138,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -187,66 +181,204 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2F3CCD-3DE1-4D13-AD96-4E84CCAA0BEB}">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,84 +712,84 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="H2" s="3" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="H2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
-        <v>18</v>
+      <c r="B3" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="H3" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
     </row>
     <row r="4" spans="2:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="H5" s="3" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="H5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
     </row>
     <row r="6" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>17</v>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="H6" s="6" t="s">
-        <v>10</v>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="H6" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
@@ -665,15 +797,15 @@
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="H7" s="6" t="s">
-        <v>11</v>
+      <c r="H7" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
@@ -681,15 +813,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="H8" s="9" t="s">
-        <v>12</v>
+      <c r="H8" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -697,15 +829,15 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="12"/>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="17"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="H9" s="4" t="s">
-        <v>9</v>
+      <c r="H9" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
@@ -713,15 +845,15 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="12"/>
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="17"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="H10" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -729,15 +861,15 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="2:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="12"/>
+      <c r="B11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="17"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="H11" s="4" t="s">
-        <v>14</v>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
@@ -745,97 +877,93 @@
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="12"/>
+      <c r="B12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="17"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="H12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="H13" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="H13" s="3"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
-      <c r="H18" s="8"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
@@ -847,7 +975,7 @@
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
@@ -859,7 +987,7 @@
       <c r="L20" s="13"/>
     </row>
     <row r="21" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -871,32 +999,32 @@
       <c r="L21" s="13"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="H23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="H28" s="3"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="H29" s="3"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
@@ -911,46 +1039,46 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
     <mergeCell ref="I17:L17"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="I13:L13"/>
     <mergeCell ref="I14:L14"/>
     <mergeCell ref="I15:L15"/>
     <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Entregable 3 Factibilidad Tecnica
Se llego hasta la factibilidad tecnica
</commit_message>
<xml_diff>
--- a/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
+++ b/Documentacion/Entregables Para Henry/Plantilla de Referencias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROYECTO_SIGEDOC\SIGEDOC\Documentacion\Entregables Para Henry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037A64D7-EB66-4B7D-B978-4400BF8D7C3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9CEB46-3C42-4C14-9C55-FA146A5E3DBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05819A6B-DF8F-4A1E-9F97-98F9155DCADB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>REQUERIMIENTO</t>
   </si>
@@ -94,13 +94,43 @@
   </si>
   <si>
     <t>Consultar rol</t>
+  </si>
+  <si>
+    <t>Objeto</t>
+  </si>
+  <si>
+    <t>Detalles</t>
+  </si>
+  <si>
+    <t>Procesador</t>
+  </si>
+  <si>
+    <t>Intel Dual Core</t>
+  </si>
+  <si>
+    <t>Memoria RAM</t>
+  </si>
+  <si>
+    <t>Disco Duro</t>
+  </si>
+  <si>
+    <t>Sistema Operativo</t>
+  </si>
+  <si>
+    <t>Windows 10 64bits</t>
+  </si>
+  <si>
+    <t>1TB</t>
+  </si>
+  <si>
+    <t>8GB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,14 +153,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -284,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -320,27 +363,45 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -359,26 +420,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,15 +746,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2F3CCD-3DE1-4D13-AD96-4E84CCAA0BEB}">
-  <dimension ref="B2:L30"/>
+  <dimension ref="B2:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:L11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" customWidth="1"/>
     <col min="8" max="8" width="27.28515625" customWidth="1"/>
     <col min="12" max="12" width="27.28515625" customWidth="1"/>
@@ -712,179 +765,179 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
       <c r="H2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="25"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="H3" s="29" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="H3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="22"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="28"/>
     </row>
     <row r="4" spans="2:12" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="25"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="H5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
       <c r="H6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
       <c r="H7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
       <c r="H8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
     </row>
     <row r="9" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
       <c r="H9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
       <c r="H10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" spans="2:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
       <c r="H11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="H12" s="31"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
@@ -892,111 +945,111 @@
     </row>
     <row r="13" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
     </row>
     <row r="15" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
     </row>
     <row r="16" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="17" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
     </row>
     <row r="18" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
     </row>
     <row r="19" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
     </row>
     <row r="20" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="2:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
@@ -1037,14 +1090,75 @@
         <v>3</v>
       </c>
     </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C20:F20"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
@@ -1052,33 +1166,12 @@
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>